<commit_message>
Some changes on report and png
</commit_message>
<xml_diff>
--- a/dadosProjeto.xlsx
+++ b/dadosProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 ano\2 semestre\CAL\Projeto\feup-cal-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E27CA5-F3C0-4598-B47C-1902A13E8894}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6491A6-5171-4AAE-B4A1-2C309F31A5AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2191EC9-5E49-4047-8E7F-8FB4B450290D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="29">
   <si>
     <t>Nodes</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>NN</t>
+  </si>
+  <si>
+    <t>Dijkstra:</t>
   </si>
 </sst>
 </file>
@@ -5736,8 +5739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6A995E-CD29-4310-804D-26025364E289}">
   <dimension ref="A2:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M78" sqref="M78"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6926,8 +6929,156 @@
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="A66" t="s">
+        <v>28</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="B67">
+        <v>19.959</v>
+      </c>
+      <c r="C67">
+        <v>114.732</v>
+      </c>
+      <c r="D67">
+        <v>30.884699999999999</v>
+      </c>
+      <c r="E67">
+        <v>96.261200000000002</v>
+      </c>
+      <c r="F67">
+        <v>3693.31</v>
+      </c>
+      <c r="G67">
+        <v>2478.59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="B68">
+        <v>28.923999999999999</v>
+      </c>
+      <c r="C68">
+        <v>84.806899999999999</v>
+      </c>
+      <c r="D68">
+        <v>24.933199999999999</v>
+      </c>
+      <c r="E68">
+        <v>286.90800000000002</v>
+      </c>
+      <c r="F68">
+        <v>3638.23</v>
+      </c>
+      <c r="G68">
+        <v>3857.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="B69">
+        <v>22.9391</v>
+      </c>
+      <c r="C69">
+        <v>103.42700000000001</v>
+      </c>
+      <c r="D69">
+        <v>19.947600000000001</v>
+      </c>
+      <c r="E69">
+        <v>101.904</v>
+      </c>
+      <c r="F69">
+        <v>3307.27</v>
+      </c>
+      <c r="G69">
+        <v>2505.56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70">
+        <v>24.932400000000001</v>
+      </c>
+      <c r="C70">
+        <v>101.52800000000001</v>
+      </c>
+      <c r="D70">
+        <v>24.965800000000002</v>
+      </c>
+      <c r="E70">
+        <v>124.667</v>
+      </c>
+      <c r="F70">
+        <v>4043.88</v>
+      </c>
+      <c r="G70">
+        <v>3041.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71">
+        <v>29.9541</v>
+      </c>
+      <c r="C71">
+        <v>110.739</v>
+      </c>
+      <c r="D71">
+        <v>16.966000000000001</v>
+      </c>
+      <c r="E71">
+        <v>87.535300000000007</v>
+      </c>
+      <c r="F71">
+        <v>4716.62</v>
+      </c>
+      <c r="G71">
+        <v>4224.71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <f t="shared" ref="B72" si="13">SUM(B67:B71)/5</f>
+        <v>25.341719999999999</v>
+      </c>
+      <c r="C72">
+        <f t="shared" ref="C72" si="14">SUM(C67:C71)/5</f>
+        <v>103.04658000000002</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ref="D72" si="15">SUM(D67:D71)/5</f>
+        <v>23.539460000000002</v>
+      </c>
+      <c r="E72">
+        <f t="shared" ref="E72" si="16">SUM(E67:E71)/5</f>
+        <v>139.45510000000002</v>
+      </c>
+      <c r="F72">
+        <f t="shared" ref="F72" si="17">SUM(F67:F71)/5</f>
+        <v>3879.8619999999996</v>
+      </c>
+      <c r="G72">
+        <f t="shared" ref="G72" si="18">SUM(G67:G71)/5</f>
+        <v>3221.5519999999997</v>
+      </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
@@ -6997,27 +7148,27 @@
         <v>24</v>
       </c>
       <c r="B81">
-        <f t="shared" ref="B81" si="13">SUM(B76:B80)/5</f>
+        <f t="shared" ref="B81" si="19">SUM(B76:B80)/5</f>
         <v>0</v>
       </c>
       <c r="C81">
-        <f t="shared" ref="C81" si="14">SUM(C76:C80)/5</f>
+        <f t="shared" ref="C81" si="20">SUM(C76:C80)/5</f>
         <v>0</v>
       </c>
       <c r="D81">
-        <f t="shared" ref="D81" si="15">SUM(D76:D80)/5</f>
+        <f t="shared" ref="D81" si="21">SUM(D76:D80)/5</f>
         <v>0</v>
       </c>
       <c r="E81">
-        <f t="shared" ref="E81" si="16">SUM(E76:E80)/5</f>
+        <f t="shared" ref="E81" si="22">SUM(E76:E80)/5</f>
         <v>0</v>
       </c>
       <c r="F81">
-        <f t="shared" ref="F81" si="17">SUM(F76:F80)/5</f>
+        <f t="shared" ref="F81" si="23">SUM(F76:F80)/5</f>
         <v>59.8</v>
       </c>
       <c r="G81">
-        <f t="shared" ref="G81" si="18">SUM(G76:G80)/5</f>
+        <f t="shared" ref="G81" si="24">SUM(G76:G80)/5</f>
         <v>175.2</v>
       </c>
     </row>
@@ -7147,7 +7298,7 @@
         <v>7938</v>
       </c>
       <c r="L89">
-        <f t="shared" ref="L89:L93" si="19">(J89+K89)*LOG(J89, 2)</f>
+        <f t="shared" ref="L89:L93" si="25">(J89+K89)*LOG(J89, 2)</f>
         <v>192516.99997686752</v>
       </c>
       <c r="M89">
@@ -7183,7 +7334,7 @@
         <v>10916</v>
       </c>
       <c r="L90">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>283876.46294730745</v>
       </c>
       <c r="M90">
@@ -7219,7 +7370,7 @@
         <v>19260</v>
       </c>
       <c r="L91">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>522792.53595200245</v>
       </c>
       <c r="M91">
@@ -7231,27 +7382,27 @@
         <v>24</v>
       </c>
       <c r="B92">
-        <f t="shared" ref="B92" si="20">SUM(B87:B91)/5</f>
+        <f t="shared" ref="B92" si="26">SUM(B87:B91)/5</f>
         <v>11.8</v>
       </c>
       <c r="C92">
-        <f t="shared" ref="C92" si="21">SUM(C87:C91)/5</f>
+        <f t="shared" ref="C92" si="27">SUM(C87:C91)/5</f>
         <v>24.6</v>
       </c>
       <c r="D92">
-        <f t="shared" ref="D92" si="22">SUM(D87:D91)/5</f>
+        <f t="shared" ref="D92" si="28">SUM(D87:D91)/5</f>
         <v>27.6</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92" si="23">SUM(E87:E91)/5</f>
+        <f t="shared" ref="E92" si="29">SUM(E87:E91)/5</f>
         <v>56.4</v>
       </c>
       <c r="F92">
-        <f t="shared" ref="F92" si="24">SUM(F87:F91)/5</f>
+        <f t="shared" ref="F92" si="30">SUM(F87:F91)/5</f>
         <v>120.2</v>
       </c>
       <c r="G92">
-        <f t="shared" ref="G92" si="25">SUM(G87:G91)/5</f>
+        <f t="shared" ref="G92" si="31">SUM(G87:G91)/5</f>
         <v>211.4</v>
       </c>
       <c r="I92" t="s">
@@ -7264,7 +7415,7 @@
         <v>29488</v>
       </c>
       <c r="L92">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>815538.42754767986</v>
       </c>
       <c r="M92">
@@ -7282,7 +7433,7 @@
         <v>59526</v>
       </c>
       <c r="L93">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>1777597.1320562561</v>
       </c>
       <c r="M93">

</xml_diff>

<commit_message>
Dados Excel mudados e graficos adicionados
</commit_message>
<xml_diff>
--- a/dadosProjeto.xlsx
+++ b/dadosProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 ano\2 semestre\CAL\Projeto\feup-cal-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6491A6-5171-4AAE-B4A1-2C309F31A5AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3353FF-EFCD-4660-9744-F9B56421E04F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2191EC9-5E49-4047-8E7F-8FB4B450290D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="31">
   <si>
     <t>Nodes</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Dijkstra:</t>
+  </si>
+  <si>
+    <t>Dijkstra</t>
+  </si>
+  <si>
+    <t>Astar</t>
   </si>
 </sst>
 </file>
@@ -687,6 +693,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42210319814475239"/>
+          <c:y val="1.1990407673860911E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -723,10 +737,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.301436557071587E-2"/>
-          <c:y val="9.9227771805277101E-2"/>
-          <c:w val="0.86486351706036746"/>
-          <c:h val="0.72088764946048411"/>
+          <c:x val="0.11155327544673355"/>
+          <c:y val="0.16517494665684776"/>
+          <c:w val="0.83061697767231157"/>
+          <c:h val="0.67892142978530556"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2475,6 +2489,922 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Dijkstra</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15436222646082284"/>
+          <c:y val="0.20238532110091745"/>
+          <c:w val="0.75260809790080585"/>
+          <c:h val="0.56884827469960753"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$L$67:$L$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>98024.430968176399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192516.99997686752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283876.46294730745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522792.53595200245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>815538.42754767986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1777597.1320562561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$M$67:$M$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>133.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3B6-4F3D-B782-1F00559552F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="531969247"/>
+        <c:axId val="531966751"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="531969247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>(|V|+|E|)*Log(|V|)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531966751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="531966751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="531969247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Astar</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$L$77:$L$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>98024.430968176399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192516.99997686752</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283876.46294730745</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>522792.53595200245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>815538.42754767986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1777597.1320562561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$M$77:$M$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-950C-42D9-BE86-E2D293784382}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="534402879"/>
+        <c:axId val="534403711"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="534402879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>(|V|+|E|)*Log(|V|)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="534403711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="534403711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="534402879"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2675,6 +3605,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5255,20 +6265,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5295,16 +7337,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5331,16 +7373,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5367,15 +7409,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>102870</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>34290</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5403,16 +7445,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5432,6 +7474,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD795741-4913-469E-A19E-0C9F95D71E9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C584EE-9F51-4DE8-84AB-98390DB2AB54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5739,8 +7853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6A995E-CD29-4310-804D-26025364E289}">
   <dimension ref="A2:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6928,7 +9042,12 @@
         <v>3221.5520000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="65" spans="1:13">
+      <c r="I65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -6950,137 +9069,248 @@
       <c r="G66" t="s">
         <v>20</v>
       </c>
+      <c r="I66" t="s">
+        <v>5</v>
+      </c>
+      <c r="J66" t="s">
+        <v>0</v>
+      </c>
+      <c r="K66" t="s">
+        <v>1</v>
+      </c>
+      <c r="L66" t="s">
+        <v>10</v>
+      </c>
+      <c r="M66" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:13">
       <c r="B67">
-        <v>19.959</v>
+        <v>9</v>
       </c>
       <c r="C67">
-        <v>114.732</v>
+        <v>15</v>
       </c>
       <c r="D67">
-        <v>30.884699999999999</v>
+        <v>17</v>
       </c>
       <c r="E67">
-        <v>96.261200000000002</v>
+        <v>34</v>
       </c>
       <c r="F67">
-        <v>3693.31</v>
+        <v>76</v>
       </c>
       <c r="G67">
-        <v>2478.59</v>
+        <v>137</v>
+      </c>
+      <c r="I67" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="1">
+        <v>3964</v>
+      </c>
+      <c r="K67" s="1">
+        <v>4237</v>
+      </c>
+      <c r="L67">
+        <f>(J67+K67)*LOG(J67, 2)</f>
+        <v>98024.430968176399</v>
+      </c>
+      <c r="M67">
+        <v>6.8</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:13">
       <c r="B68">
-        <v>28.923999999999999</v>
+        <v>5</v>
       </c>
       <c r="C68">
-        <v>84.806899999999999</v>
+        <v>14</v>
       </c>
       <c r="D68">
-        <v>24.933199999999999</v>
+        <v>18</v>
       </c>
       <c r="E68">
-        <v>286.90800000000002</v>
+        <v>35</v>
       </c>
       <c r="F68">
-        <v>3638.23</v>
+        <v>73</v>
       </c>
       <c r="G68">
-        <v>3857.6</v>
+        <v>133</v>
+      </c>
+      <c r="I68" t="s">
+        <v>12</v>
+      </c>
+      <c r="J68" s="1">
+        <v>7108</v>
+      </c>
+      <c r="K68" s="1">
+        <v>7938</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L72" si="13">(J68+K68)*LOG(J68, 2)</f>
+        <v>192516.99997686752</v>
+      </c>
+      <c r="M68">
+        <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:13">
       <c r="B69">
-        <v>22.9391</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>103.42700000000001</v>
+        <v>21</v>
       </c>
       <c r="D69">
-        <v>19.947600000000001</v>
+        <v>16</v>
       </c>
       <c r="E69">
-        <v>101.904</v>
+        <v>38</v>
       </c>
       <c r="F69">
-        <v>3307.27</v>
+        <v>78</v>
       </c>
       <c r="G69">
-        <v>2505.56</v>
+        <v>136</v>
+      </c>
+      <c r="I69" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69" s="1">
+        <v>10365</v>
+      </c>
+      <c r="K69" s="1">
+        <v>10916</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="13"/>
+        <v>283876.46294730745</v>
+      </c>
+      <c r="M69">
+        <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:13">
       <c r="B70">
-        <v>24.932400000000001</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>101.52800000000001</v>
+        <v>17</v>
       </c>
       <c r="D70">
-        <v>24.965800000000002</v>
+        <v>16</v>
       </c>
       <c r="E70">
-        <v>124.667</v>
+        <v>37</v>
       </c>
       <c r="F70">
-        <v>4043.88</v>
+        <v>74</v>
       </c>
       <c r="G70">
-        <v>3041.3</v>
+        <v>130</v>
+      </c>
+      <c r="I70" t="s">
+        <v>2</v>
+      </c>
+      <c r="J70" s="1">
+        <v>17772</v>
+      </c>
+      <c r="K70" s="1">
+        <v>19260</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="13"/>
+        <v>522792.53595200245</v>
+      </c>
+      <c r="M70">
+        <v>35.6</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:13">
       <c r="B71">
-        <v>29.9541</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>110.739</v>
+        <v>16</v>
       </c>
       <c r="D71">
-        <v>16.966000000000001</v>
+        <v>16</v>
       </c>
       <c r="E71">
-        <v>87.535300000000007</v>
+        <v>34</v>
       </c>
       <c r="F71">
-        <v>4716.62</v>
+        <v>79</v>
       </c>
       <c r="G71">
-        <v>4224.71</v>
+        <v>132</v>
+      </c>
+      <c r="I71" t="s">
+        <v>13</v>
+      </c>
+      <c r="J71" s="1">
+        <v>26098</v>
+      </c>
+      <c r="K71" s="1">
+        <v>29488</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="13"/>
+        <v>815538.42754767986</v>
+      </c>
+      <c r="M71">
+        <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>24</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="B72" si="13">SUM(B67:B71)/5</f>
-        <v>25.341719999999999</v>
+        <f t="shared" ref="B72" si="14">SUM(B67:B71)/5</f>
+        <v>6.8</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72" si="14">SUM(C67:C71)/5</f>
-        <v>103.04658000000002</v>
+        <f t="shared" ref="C72" si="15">SUM(C67:C71)/5</f>
+        <v>16.600000000000001</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72" si="15">SUM(D67:D71)/5</f>
-        <v>23.539460000000002</v>
+        <f t="shared" ref="D72" si="16">SUM(D67:D71)/5</f>
+        <v>16.600000000000001</v>
       </c>
       <c r="E72">
-        <f t="shared" ref="E72" si="16">SUM(E67:E71)/5</f>
-        <v>139.45510000000002</v>
+        <f t="shared" ref="E72" si="17">SUM(E67:E71)/5</f>
+        <v>35.6</v>
       </c>
       <c r="F72">
-        <f t="shared" ref="F72" si="17">SUM(F67:F71)/5</f>
-        <v>3879.8619999999996</v>
+        <f t="shared" ref="F72" si="18">SUM(F67:F71)/5</f>
+        <v>76</v>
       </c>
       <c r="G72">
-        <f t="shared" ref="G72" si="18">SUM(G67:G71)/5</f>
-        <v>3221.5519999999997</v>
+        <f t="shared" ref="G72" si="19">SUM(G67:G71)/5</f>
+        <v>133.6</v>
+      </c>
+      <c r="I72" t="s">
+        <v>3</v>
+      </c>
+      <c r="J72" s="1">
+        <v>53621</v>
+      </c>
+      <c r="K72" s="1">
+        <v>59526</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="13"/>
+        <v>1777597.1320562561</v>
+      </c>
+      <c r="M72">
+        <v>133.6</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -7102,45 +9332,187 @@
       <c r="G75" t="s">
         <v>20</v>
       </c>
+      <c r="I75" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:13">
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>19</v>
+      </c>
+      <c r="E76">
+        <v>33</v>
+      </c>
       <c r="F76">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G76">
-        <v>174</v>
+        <v>198</v>
+      </c>
+      <c r="I76" t="s">
+        <v>5</v>
+      </c>
+      <c r="J76" t="s">
+        <v>0</v>
+      </c>
+      <c r="K76" t="s">
+        <v>1</v>
+      </c>
+      <c r="L76" t="s">
+        <v>10</v>
+      </c>
+      <c r="M76" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:13">
+      <c r="B77">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>17</v>
+      </c>
+      <c r="D77">
+        <v>18</v>
+      </c>
+      <c r="E77">
+        <v>33</v>
+      </c>
       <c r="F77">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G77">
-        <v>176</v>
+        <v>192</v>
+      </c>
+      <c r="I77" t="s">
+        <v>11</v>
+      </c>
+      <c r="J77" s="1">
+        <v>3964</v>
+      </c>
+      <c r="K77" s="1">
+        <v>4237</v>
+      </c>
+      <c r="L77">
+        <f>(J77+K77)*LOG(J77, 2)</f>
+        <v>98024.430968176399</v>
+      </c>
+      <c r="M77">
+        <v>6.6</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:13">
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>16</v>
+      </c>
+      <c r="D78">
+        <v>19</v>
+      </c>
+      <c r="E78">
+        <v>32</v>
+      </c>
       <c r="F78">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G78">
-        <v>173</v>
+        <v>196</v>
+      </c>
+      <c r="I78" t="s">
+        <v>12</v>
+      </c>
+      <c r="J78" s="1">
+        <v>7108</v>
+      </c>
+      <c r="K78" s="1">
+        <v>7938</v>
+      </c>
+      <c r="L78">
+        <f t="shared" ref="L78:L82" si="20">(J78+K78)*LOG(J78, 2)</f>
+        <v>192516.99997686752</v>
+      </c>
+      <c r="M78">
+        <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:13">
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79">
+        <v>16</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <v>32</v>
+      </c>
       <c r="F79">
         <v>61</v>
       </c>
       <c r="G79">
-        <v>176</v>
+        <v>202</v>
+      </c>
+      <c r="I79" t="s">
+        <v>6</v>
+      </c>
+      <c r="J79" s="1">
+        <v>10365</v>
+      </c>
+      <c r="K79" s="1">
+        <v>10916</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="20"/>
+        <v>283876.46294730745</v>
+      </c>
+      <c r="M79">
+        <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:13">
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>19</v>
+      </c>
+      <c r="E80">
+        <v>33</v>
+      </c>
       <c r="F80">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G80">
-        <v>177</v>
+        <v>196</v>
+      </c>
+      <c r="I80" t="s">
+        <v>2</v>
+      </c>
+      <c r="J80" s="1">
+        <v>17772</v>
+      </c>
+      <c r="K80" s="1">
+        <v>19260</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="20"/>
+        <v>522792.53595200245</v>
+      </c>
+      <c r="M80">
+        <v>32.6</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -7148,28 +9520,62 @@
         <v>24</v>
       </c>
       <c r="B81">
-        <f t="shared" ref="B81" si="19">SUM(B76:B80)/5</f>
-        <v>0</v>
+        <f t="shared" ref="B81" si="21">SUM(B76:B80)/5</f>
+        <v>6.6</v>
       </c>
       <c r="C81">
-        <f t="shared" ref="C81" si="20">SUM(C76:C80)/5</f>
-        <v>0</v>
+        <f>SUM(C76:C80)/5</f>
+        <v>16</v>
       </c>
       <c r="D81">
-        <f t="shared" ref="D81" si="21">SUM(D76:D80)/5</f>
-        <v>0</v>
+        <f>SUM(D76:D80)/5</f>
+        <v>19</v>
       </c>
       <c r="E81">
         <f t="shared" ref="E81" si="22">SUM(E76:E80)/5</f>
-        <v>0</v>
+        <v>32.6</v>
       </c>
       <c r="F81">
         <f t="shared" ref="F81" si="23">SUM(F76:F80)/5</f>
-        <v>59.8</v>
+        <v>63.8</v>
       </c>
       <c r="G81">
         <f t="shared" ref="G81" si="24">SUM(G76:G80)/5</f>
-        <v>175.2</v>
+        <v>196.8</v>
+      </c>
+      <c r="I81" t="s">
+        <v>13</v>
+      </c>
+      <c r="J81" s="1">
+        <v>26098</v>
+      </c>
+      <c r="K81" s="1">
+        <v>29488</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="20"/>
+        <v>815538.42754767986</v>
+      </c>
+      <c r="M81">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="I82" t="s">
+        <v>3</v>
+      </c>
+      <c r="J82" s="1">
+        <v>53621</v>
+      </c>
+      <c r="K82" s="1">
+        <v>59526</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="20"/>
+        <v>1777597.1320562561</v>
+      </c>
+      <c r="M82">
+        <v>196.8</v>
       </c>
     </row>
     <row r="86" spans="1:13">

</xml_diff>

<commit_message>
New Excel data and changes on report algo implemented
</commit_message>
<xml_diff>
--- a/dadosProjeto.xlsx
+++ b/dadosProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 ano\2 semestre\CAL\Projeto\feup-cal-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3353FF-EFCD-4660-9744-F9B56421E04F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D41E692-AB98-4993-961E-BCB0AC48FA03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2191EC9-5E49-4047-8E7F-8FB4B450290D}"/>
   </bookViews>
@@ -2252,7 +2252,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT"/>
-                  <a:t>(|V|+|E|)*log(|V|)</a:t>
+                  <a:t>|POI|*((|V|+|E|)*log(|V|))</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7853,8 +7853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6A995E-CD29-4310-804D-26025364E289}">
   <dimension ref="A2:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W94" sqref="W94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Solution of Problem on Report
</commit_message>
<xml_diff>
--- a/dadosProjeto.xlsx
+++ b/dadosProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 ano\2 semestre\CAL\Projeto\feup-cal-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9569EB7-C427-4861-8AD8-F1CAEE632D79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C2A50-D073-4667-824F-ECFCF75F4124}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2191EC9-5E49-4047-8E7F-8FB4B450290D}"/>
   </bookViews>
@@ -3624,7 +3624,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT"/>
-                  <a:t>(|V|+|E|)*log(|V|)</a:t>
+                  <a:t>|POI|*(|V|+|E|)*log(|V|)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8901,8 +8901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6A995E-CD29-4310-804D-26025364E289}">
   <dimension ref="A2:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W106" sqref="W106"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10917,7 +10917,7 @@
         <v>20</v>
       </c>
       <c r="I101" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="102" spans="1:13">

</xml_diff>

<commit_message>
Spacial complexity added to Report
</commit_message>
<xml_diff>
--- a/dadosProjeto.xlsx
+++ b/dadosProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 ano\2 semestre\CAL\Projeto\feup-cal-proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30C2A50-D073-4667-824F-ECFCF75F4124}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4173B4EC-E86A-4402-8254-C124DF9A7F88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2191EC9-5E49-4047-8E7F-8FB4B450290D}"/>
   </bookViews>
@@ -3624,7 +3624,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT"/>
-                  <a:t>|POI|*(|V|+|E|)*log(|V|)</a:t>
+                  <a:t>log|POI|*|POI|*(|V|+|E|)*log|V|</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8902,7 +8902,7 @@
   <dimension ref="A2:M108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M110" sqref="M110"/>
+      <selection activeCell="W103" sqref="W103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>